<commit_message>
Changed percentages and rerun
</commit_message>
<xml_diff>
--- a/notebooks/eur_clas.xlsx
+++ b/notebooks/eur_clas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,58 +547,58 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.866</v>
+        <v>0.91</v>
       </c>
       <c r="C2" t="n">
-        <v>0.699</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0.636</v>
+        <v>0.629</v>
       </c>
       <c r="E2" t="n">
-        <v>0.899</v>
+        <v>0.9320000000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>0.77</v>
+        <v>0.769</v>
       </c>
       <c r="G2" t="n">
-        <v>0.726</v>
+        <v>0.721</v>
       </c>
       <c r="H2" t="n">
-        <v>0.46</v>
+        <v>0.383</v>
       </c>
       <c r="I2" t="n">
-        <v>0.735</v>
+        <v>0.736</v>
       </c>
       <c r="J2" t="n">
-        <v>0.803</v>
+        <v>0.849</v>
       </c>
       <c r="K2" t="n">
-        <v>0.137</v>
+        <v>0.091</v>
       </c>
       <c r="L2" t="n">
-        <v>0.33</v>
+        <v>0.329</v>
       </c>
       <c r="M2" t="n">
-        <v>0.396</v>
+        <v>0.417</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1319999992847443</v>
+        <v>0.1150000020861626</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1949999928474426</v>
+        <v>0.1940000057220459</v>
       </c>
       <c r="P2" t="n">
-        <v>0.2150000035762787</v>
+        <v>0.2189999967813492</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.08600000292062759</v>
+        <v>0.07800000160932541</v>
       </c>
       <c r="R2" t="n">
-        <v>0.125</v>
+        <v>0.1209999993443489</v>
       </c>
       <c r="S2" t="n">
-        <v>0.1389999985694885</v>
+        <v>0.1410000026226044</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -618,58 +618,58 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.451</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.489</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.665</v>
+      </c>
+      <c r="F3" t="n">
         <v>0.569</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.418</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.494</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.669</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.551</v>
-      </c>
       <c r="G3" t="n">
-        <v>0.612</v>
+        <v>0.61</v>
       </c>
       <c r="H3" t="n">
-        <v>0.823</v>
+        <v>0.849</v>
       </c>
       <c r="I3" t="n">
-        <v>0.976</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J3" t="n">
-        <v>0.944</v>
+        <v>0.975</v>
       </c>
       <c r="K3" t="n">
-        <v>0.442</v>
+        <v>0.46</v>
       </c>
       <c r="L3" t="n">
-        <v>0.615</v>
+        <v>0.579</v>
       </c>
       <c r="M3" t="n">
-        <v>0.548</v>
+        <v>0.569</v>
       </c>
       <c r="N3" t="n">
-        <v>0.210999995470047</v>
+        <v>0.2169999927282333</v>
       </c>
       <c r="O3" t="n">
-        <v>0.25</v>
+        <v>0.2370000034570694</v>
       </c>
       <c r="P3" t="n">
-        <v>0.2419999986886978</v>
+        <v>0.2479999959468842</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1439999938011169</v>
+        <v>0.1490000039339066</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1780000030994415</v>
+        <v>0.1650000065565109</v>
       </c>
       <c r="S3" t="n">
-        <v>0.1689999997615814</v>
+        <v>0.1739999949932098</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
@@ -685,208 +685,208 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>40_sage</t>
+          <t>75_gat</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.975</v>
+        <v>0.424</v>
       </c>
       <c r="C4" t="n">
-        <v>0.613</v>
+        <v>0.443</v>
       </c>
       <c r="D4" t="n">
-        <v>0.571</v>
+        <v>0.459</v>
       </c>
       <c r="E4" t="n">
-        <v>0.982</v>
+        <v>0.551</v>
       </c>
       <c r="F4" t="n">
-        <v>0.708</v>
+        <v>0.569</v>
       </c>
       <c r="G4" t="n">
-        <v>0.678</v>
+        <v>0.577</v>
       </c>
       <c r="H4" t="n">
-        <v>0.18</v>
+        <v>1.42</v>
       </c>
       <c r="I4" t="n">
-        <v>0.997</v>
+        <v>1.442</v>
       </c>
       <c r="J4" t="n">
-        <v>0.973</v>
+        <v>1.349</v>
       </c>
       <c r="K4" t="n">
-        <v>0.023</v>
+        <v>0.888</v>
       </c>
       <c r="L4" t="n">
-        <v>0.493</v>
+        <v>0.894</v>
       </c>
       <c r="M4" t="n">
-        <v>0.513</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="N4" t="n">
-        <v>0.08100000023841858</v>
+        <v>0.363999992609024</v>
       </c>
       <c r="O4" t="n">
-        <v>0.2560000121593475</v>
+        <v>0.3759999871253967</v>
       </c>
       <c r="P4" t="n">
-        <v>0.25</v>
+        <v>0.3569999933242798</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.06599999964237213</v>
+        <v>0.2529999911785126</v>
       </c>
       <c r="R4" t="n">
-        <v>0.1560000032186508</v>
+        <v>0.2590000033378601</v>
       </c>
       <c r="S4" t="n">
-        <v>0.1650000065565109</v>
+        <v>0.2450000047683716</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>75</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>sage</t>
+          <t>gat</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>40_fnn</t>
+          <t>75_gcn</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.528</v>
+        <v>0.269</v>
       </c>
       <c r="C5" t="n">
-        <v>0.556</v>
+        <v>0.339</v>
       </c>
       <c r="D5" t="n">
-        <v>0.482</v>
+        <v>0.254</v>
       </c>
       <c r="E5" t="n">
-        <v>0.644</v>
+        <v>0.403</v>
       </c>
       <c r="F5" t="n">
-        <v>0.667</v>
+        <v>0.491</v>
       </c>
       <c r="G5" t="n">
-        <v>0.607</v>
+        <v>0.395</v>
       </c>
       <c r="H5" t="n">
-        <v>0.869</v>
+        <v>1.49</v>
       </c>
       <c r="I5" t="n">
-        <v>0.898</v>
+        <v>1.445</v>
       </c>
       <c r="J5" t="n">
-        <v>0.967</v>
+        <v>1.513</v>
       </c>
       <c r="K5" t="n">
-        <v>0.487</v>
+        <v>1.052</v>
       </c>
       <c r="L5" t="n">
-        <v>0.486</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="M5" t="n">
-        <v>0.5649999999999999</v>
+        <v>1.08</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2189999967813492</v>
+        <v>0.3680000007152557</v>
       </c>
       <c r="O5" t="n">
-        <v>0.2409999966621399</v>
+        <v>0.3630000054836273</v>
       </c>
       <c r="P5" t="n">
-        <v>0.2430000007152557</v>
+        <v>0.3819999992847443</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.1519999951124191</v>
+        <v>0.2829999923706055</v>
       </c>
       <c r="R5" t="n">
-        <v>0.1620000004768372</v>
+        <v>0.2630000114440918</v>
       </c>
       <c r="S5" t="n">
-        <v>0.1679999977350235</v>
+        <v>0.2960000038146973</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>75</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>fnn</t>
+          <t>gcn</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>10_sage</t>
+          <t>40_sage</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.987</v>
+        <v>0.974</v>
       </c>
       <c r="C6" t="n">
-        <v>0.662</v>
+        <v>0.613</v>
       </c>
       <c r="D6" t="n">
-        <v>0.509</v>
+        <v>0.578</v>
       </c>
       <c r="E6" t="n">
-        <v>0.99</v>
+        <v>0.981</v>
       </c>
       <c r="F6" t="n">
-        <v>0.744</v>
+        <v>0.713</v>
       </c>
       <c r="G6" t="n">
-        <v>0.63</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1</v>
+        <v>0.14</v>
       </c>
       <c r="I6" t="n">
-        <v>0.849</v>
+        <v>0.928</v>
       </c>
       <c r="J6" t="n">
-        <v>1.123</v>
+        <v>0.957</v>
       </c>
       <c r="K6" t="n">
-        <v>0.01</v>
+        <v>0.019</v>
       </c>
       <c r="L6" t="n">
-        <v>0.395</v>
+        <v>0.461</v>
       </c>
       <c r="M6" t="n">
-        <v>0.633</v>
+        <v>0.507</v>
       </c>
       <c r="N6" t="n">
-        <v>0.07599999755620956</v>
+        <v>0.07500000298023224</v>
       </c>
       <c r="O6" t="n">
-        <v>0.2129999995231628</v>
+        <v>0.2360000014305115</v>
       </c>
       <c r="P6" t="n">
-        <v>0.2849999964237213</v>
+        <v>0.2479999959468842</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.06599999964237213</v>
+        <v>0.06300000101327896</v>
       </c>
       <c r="R6" t="n">
-        <v>0.1280000060796738</v>
+        <v>0.1500000059604645</v>
       </c>
       <c r="S6" t="n">
-        <v>0.1920000016689301</v>
+        <v>0.164000004529953</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>40</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -898,71 +898,497 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
+          <t>40_fnn</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.576</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.494</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.6870000000000001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.616</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.786</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.928</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.489</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.409</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.537</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.2240000069141388</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.2129999995231628</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.2360000014305115</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.153999999165535</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.1420000046491623</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.164000004529953</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>fnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>40_gat</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.466</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.589</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.617</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.541</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.217</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.244</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.318</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.829</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.3109999895095825</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.3109999895095825</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.3310000002384186</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.210999995470047</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.2060000002384186</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.2339999973773956</v>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>gat</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>40_gcn</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.278</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.276</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.346</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.287</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.361</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.164</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.146</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.198</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.887</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.913</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.904</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.2899999916553497</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.289000004529953</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.3009999990463257</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.2349999994039536</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.2419999986886978</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.2419999986886978</v>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>gcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
           <t>10_fnn</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>0.648</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.531</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.443</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.733</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="B10" t="n">
         <v>0.651</v>
       </c>
-      <c r="G7" t="n">
-        <v>0.573</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.724</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.876</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.982</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.347</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.488</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.1829999983310699</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.2070000022649765</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0.2489999979734421</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="R7" t="n">
-        <v>0.1430000066757202</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0.1770000010728836</v>
-      </c>
-      <c r="T7" t="inlineStr">
+      <c r="C10" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.463</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.739</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.714</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.734</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.707</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.958</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.348</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.357</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.574</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.1870000064373016</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.1630000025033951</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.2430000007152557</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.1280000060796738</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.1150000020861626</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.1710000038146973</v>
+      </c>
+      <c r="T10" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr">
+      <c r="U10" t="inlineStr">
         <is>
           <t>fnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>10_sage</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.977</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.534</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.983</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.594</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.132</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1.035</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.216</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.719</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.07800000160932541</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.2590000033378601</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.3050000071525574</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.06700000166893005</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.1700000017881393</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.2080000042915344</v>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>sage</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>10_gat</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.374</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.271</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.319</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.464</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.468</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.345</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.488</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1.515</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1.018</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.3459999859333038</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.3549999892711639</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.3910000026226044</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.2339999973773956</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.2630000114440918</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.2840000092983246</v>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>gat</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>10_gcn</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.193</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.021</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.374</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.214</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.313</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.134</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.512</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.459</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1.214</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1.108</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.2849999964237213</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.3689999878406525</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.3709999918937683</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.2220000028610229</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.3059999942779541</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.2949999868869781</v>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>gcn</t>
         </is>
       </c>
     </row>

</xml_diff>